<commit_message>
Visual updates to the app
</commit_message>
<xml_diff>
--- a/data/OPpayments.xlsx
+++ b/data/OPpayments.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Ai-banker/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jetroanttonen/ai-banker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="28040" windowHeight="16660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="OP" sheetId="1" r:id="rId1"/>
     <sheet name="Nordea" sheetId="2" r:id="rId2"/>
     <sheet name="Varallisuus" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -46,9 +52,6 @@
     <t>Income</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Rent</t>
   </si>
   <si>
@@ -118,12 +121,6 @@
     <t>Naughty Burger</t>
   </si>
   <si>
-    <t>Student loan</t>
-  </si>
-  <si>
-    <t>Loans</t>
-  </si>
-  <si>
     <t>Firm2</t>
   </si>
   <si>
@@ -173,12 +170,15 @@
   </si>
   <si>
     <t>Rahasto</t>
+  </si>
+  <si>
+    <t>Expenditure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -214,7 +214,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,10 +551,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -569,16 +569,16 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -590,19 +590,19 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>550</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -614,19 +614,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>330</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -638,19 +638,19 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -668,13 +668,13 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -686,19 +686,19 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -710,19 +710,19 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -734,19 +734,19 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -758,19 +758,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -782,19 +782,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -806,19 +806,19 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D12">
         <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -830,19 +830,19 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D13">
         <v>20</v>
       </c>
       <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -860,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -878,19 +878,19 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -902,19 +902,19 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>150</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -926,19 +926,19 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -950,19 +950,19 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -974,19 +974,19 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -998,19 +998,19 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1022,19 +1022,19 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D21">
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1046,19 +1046,19 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1070,19 +1070,19 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D23">
         <v>10</v>
       </c>
       <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
         <v>20</v>
       </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1094,19 +1094,19 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1118,19 +1118,19 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>70</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1142,19 +1142,19 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1166,19 +1166,19 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D27">
         <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1190,19 +1190,19 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D28">
         <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1214,19 +1214,19 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D29">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1238,19 +1238,19 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D30">
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1262,19 +1262,19 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D31">
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1286,19 +1286,19 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D32">
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1316,13 +1316,13 @@
         <v>3000</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1334,19 +1334,19 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D34">
         <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1358,19 +1358,19 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D35">
         <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1386,7 +1386,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,10 +1408,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1429,13 +1429,13 @@
         <v>500</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1447,19 +1447,19 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1471,19 +1471,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
         <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1495,19 +1495,19 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>250</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1525,13 +1525,13 @@
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1551,27 +1551,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>1400</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1579,13 +1579,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>20000</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1593,13 +1593,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>3300</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1607,13 +1607,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>160000</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -1621,13 +1621,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>100000</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>0.5</v>
@@ -1635,13 +1635,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>12000</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>0.1</v>
@@ -1649,13 +1649,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>1100</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>4</v>

</xml_diff>